<commit_message>
Added exercises 24 to 43 of Chapter 7
</commit_message>
<xml_diff>
--- a/C++_Primer/Progress.xlsx
+++ b/C++_Primer/Progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ToDo\ToDelete\C++_Primer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Programming\C++\C++_Primer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D157E1C-95C8-434B-B75F-5D9B5742E88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFE118D-A364-4C6D-B8B8-AD943997A747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{4C9C5218-05B8-4A68-B246-F8137B94F19E}"/>
   </bookViews>
@@ -19,6 +19,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -442,11 +449,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F248D4-318C-4F5E-A22D-E47D3A2A1DDD}">
-  <dimension ref="B1:H16"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -525,11 +530,11 @@
         <v>0.29652777777777778</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" ref="F4:F16" si="0">D4-C4</f>
+        <f t="shared" ref="F4:F19" si="0">D4-C4</f>
         <v>35</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G16" si="1">F4/(3*E4)</f>
+        <f t="shared" ref="G4:G19" si="1">F4/(3*E4)</f>
         <v>39.344262295081961</v>
       </c>
       <c r="H4" s="8"/>
@@ -799,6 +804,72 @@
       <c r="G16" s="11">
         <f t="shared" si="1"/>
         <v>28.822170900692839</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>44489</v>
+      </c>
+      <c r="C17" s="1">
+        <v>354</v>
+      </c>
+      <c r="D17" s="1">
+        <v>361</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>10.980392156862745</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>44495</v>
+      </c>
+      <c r="C18" s="1">
+        <v>362</v>
+      </c>
+      <c r="D18" s="1">
+        <v>366</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="1"/>
+        <v>56.470588235294116</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>44503</v>
+      </c>
+      <c r="C19" s="1">
+        <v>367</v>
+      </c>
+      <c r="D19" s="1">
+        <v>396</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.15138888888888888</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="1"/>
+        <v>63.853211009174323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>